<commit_message>
Modulo 1 y Modulo 2 completos
</commit_message>
<xml_diff>
--- a/defects/TPO - TC and Defect - PE-54.xlsx
+++ b/defects/TPO - TC and Defect - PE-54.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Aplicaciones\Proyectos\TestingAplicaciones-MatrixTesters-TPO\defects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21E3A9C-7017-4F2D-A55D-292E747052F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EEDF54-ECA1-437E-8C31-9A7E48DAD187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="1905" windowWidth="24270" windowHeight="11385" xr2:uid="{DCE1F527-8622-40D5-806A-6A7E2BCE07A3}"/>
+    <workbookView xWindow="7110" yWindow="2955" windowWidth="24270" windowHeight="11385" xr2:uid="{DCE1F527-8622-40D5-806A-6A7E2BCE07A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Defect Report - MT-12" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Title</t>
   </si>
@@ -74,40 +74,61 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Error al ingresar el mail</t>
-  </si>
-  <si>
-    <t>Debería perdir el mail y tras validarlo mostrar el formulario</t>
-  </si>
-  <si>
     <t>1- Abrir la aplicación</t>
   </si>
   <si>
     <t>2- Clic en Sign in</t>
   </si>
   <si>
-    <t>La página muestra un campo para llenar el mail</t>
-  </si>
-  <si>
-    <t>La página muestra el formulario</t>
-  </si>
-  <si>
-    <t>Incidencia - El formulario se muestra antes de validar que el mail no exista</t>
-  </si>
-  <si>
-    <t>4- Ingreso de mail</t>
-  </si>
-  <si>
-    <t>Affected User Story: MT-01</t>
-  </si>
-  <si>
     <t>QA environment, http://127.0.0.1:5000/</t>
   </si>
   <si>
-    <t>Al leer la historia de usuario se entendía que se abría una pestaña o saldría un cartel que notificaría si el mail ingresado está en uso o no.</t>
-  </si>
-  <si>
-    <t>3- Clic en Register Here</t>
+    <t>Error al bloquear al usuario</t>
+  </si>
+  <si>
+    <t>Debería informar que el usuario se encuentra bloquedo</t>
+  </si>
+  <si>
+    <t>4- Completar campo "Password"</t>
+  </si>
+  <si>
+    <t>3- Completar campo "Email address"</t>
+  </si>
+  <si>
+    <t>5- Clic en Sign in</t>
+  </si>
+  <si>
+    <t>6- Completar campo "Email address"</t>
+  </si>
+  <si>
+    <t>7- Completar campo "Password"</t>
+  </si>
+  <si>
+    <t>8- Clic en Sign in</t>
+  </si>
+  <si>
+    <t>9- Completar campo "Email address"</t>
+  </si>
+  <si>
+    <t>10- Completar campo "Password"</t>
+  </si>
+  <si>
+    <t>11- Clic en Sign in</t>
+  </si>
+  <si>
+    <t>La página muestra "User or Password are invalid, Please try again"</t>
+  </si>
+  <si>
+    <t>La página muestra "Your user has been blockled", bloquea al usuario"</t>
+  </si>
+  <si>
+    <t>Incidencia - No se bloquea la cuenta si ingresa de forma erronea 3 veces consecutivas.</t>
+  </si>
+  <si>
+    <t>Al leer la historia de usuario se entendía que se notificaría que usuario ha sido bloqueado y que por lo tanto no podría intentar iniciar sesión otra vez.</t>
+  </si>
+  <si>
+    <t>Affected User Story: MT-11, MT-12 y MT-10</t>
   </si>
 </sst>
 </file>
@@ -639,16 +660,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19C3A39-FFB1-416B-9AA1-6DCAB5934A9A}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="67.85546875" customWidth="1"/>
+    <col min="2" max="2" width="71.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -656,7 +677,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -664,7 +685,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -672,88 +693,130 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>18</v>
+      <c r="A14" s="5"/>
+      <c r="B14" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="8" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>20</v>
+        <v>3</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="140.44999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B26" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="B28" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>22</v>
+      <c r="B30" s="13" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>